<commit_message>
Popraw literówkę w legendzie macierzy odpowiedzialności
</commit_message>
<xml_diff>
--- a/cwiczenie-2-meta/macierz-odpowiedzialnosci/figury/macierz-odpowiedzialnosci.xlsx
+++ b/cwiczenie-2-meta/macierz-odpowiedzialnosci/figury/macierz-odpowiedzialnosci.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -40,6 +40,34 @@
   </si>
   <si>
     <t>I</t>
+  </si>
+  <si>
+    <t>Tomasz
+Cudziło</t>
+  </si>
+  <si>
+    <t>Dominik
+Gebert</t>
+  </si>
+  <si>
+    <t>Łukasz
+Gwiazda</t>
+  </si>
+  <si>
+    <t>Mateusz
+Malicki</t>
+  </si>
+  <si>
+    <t>Mateusz
+Ochtera</t>
+  </si>
+  <si>
+    <t>Arkadiusz
+Osowski</t>
+  </si>
+  <si>
+    <t>Michał
+Słotwiński</t>
   </si>
   <si>
     <r>
@@ -61,38 +89,10 @@
       </rPr>
       <t xml:space="preserve">
 A = Accountable, Kierownik podzespołu
-R = Resposible, Członek zespołu
+R = Responsible, Członek zespołu
 C = Consultant, Wtyka kierownika
 I = Informed, Śledzą wyniki prac</t>
     </r>
-  </si>
-  <si>
-    <t>Tomasz
-Cudziło</t>
-  </si>
-  <si>
-    <t>Dominik
-Gebert</t>
-  </si>
-  <si>
-    <t>Łukasz
-Gwiazda</t>
-  </si>
-  <si>
-    <t>Mateusz
-Malicki</t>
-  </si>
-  <si>
-    <t>Mateusz
-Ochtera</t>
-  </si>
-  <si>
-    <t>Arkadiusz
-Osowski</t>
-  </si>
-  <si>
-    <t>Michał
-Słotwiński</t>
   </si>
 </sst>
 </file>
@@ -269,23 +269,23 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -614,40 +614,40 @@
   <cols>
     <col min="1" max="1" width="27.5" style="1" customWidth="1"/>
     <col min="2" max="2" width="1.5" style="1" customWidth="1"/>
-    <col min="3" max="9" width="13.6640625" style="1" customWidth="1"/>
+    <col min="3" max="9" width="9.83203125" style="1" customWidth="1"/>
     <col min="10" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="30" customHeight="1">
-      <c r="A1" s="13"/>
-      <c r="B1" s="13"/>
+      <c r="A1" s="11"/>
+      <c r="B1" s="11"/>
       <c r="C1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>13</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="30" customHeight="1">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="14"/>
+      <c r="B2" s="12"/>
       <c r="C2" s="4" t="s">
         <v>5</v>
       </c>
@@ -663,10 +663,10 @@
       <c r="I2" s="5"/>
     </row>
     <row r="3" spans="1:12" ht="30" customHeight="1">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="15"/>
+      <c r="B3" s="13"/>
       <c r="C3" s="9" t="s">
         <v>4</v>
       </c>
@@ -691,10 +691,10 @@
       <c r="L3" s="2"/>
     </row>
     <row r="4" spans="1:12" ht="30" customHeight="1">
-      <c r="A4" s="16" t="s">
+      <c r="A4" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="16"/>
+      <c r="B4" s="14"/>
       <c r="C4" s="10" t="s">
         <v>4</v>
       </c>
@@ -713,17 +713,17 @@
       <c r="L5" s="2"/>
     </row>
     <row r="6" spans="1:12" ht="90" customHeight="1">
-      <c r="A6" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="11"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12"/>
+      <c r="A6" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="15"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="16"/>
+      <c r="H6" s="16"/>
+      <c r="I6" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -731,8 +731,8 @@
   </mergeCells>
   <phoneticPr fontId="8" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
-  <pageMargins left="0.70000000000000007" right="0.70000000000000007" top="0.75000000000000011" bottom="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
-  <pageSetup paperSize="9" scale="98" orientation="landscape"/>
+  <pageMargins left="0.78740157480314965" right="0.78740157480314965" top="0.78740157480314965" bottom="0.78740157480314965" header="0" footer="0"/>
+  <pageSetup paperSize="9" orientation="landscape"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>